<commit_message>
base1 ci ejecucion 1
</commit_message>
<xml_diff>
--- a/output/ejecucion_1/gridsearch_results/base1/b1_ci_results_gs_rf_nrs.xlsx
+++ b/output/ejecucion_1/gridsearch_results/base1/b1_ci_results_gs_rf_nrs.xlsx
@@ -561,16 +561,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>291.792099237442</v>
+        <v>155.9807553291321</v>
       </c>
       <c r="C2">
-        <v>1.122723825608438</v>
+        <v>58.87547225374421</v>
       </c>
       <c r="D2">
-        <v>5.399229335784912</v>
+        <v>2.226694631576538</v>
       </c>
       <c r="E2">
-        <v>0.3776224339434608</v>
+        <v>3.088080238127659</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -614,16 +614,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>549.5815844535828</v>
+        <v>417.4680068969727</v>
       </c>
       <c r="C3">
-        <v>2.491825149060776</v>
+        <v>131.4527615176957</v>
       </c>
       <c r="D3">
-        <v>7.904629755020141</v>
+        <v>4.612991762161255</v>
       </c>
       <c r="E3">
-        <v>0.597394012077726</v>
+        <v>2.038105918452289</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -667,16 +667,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1075.395673894882</v>
+        <v>831.4452156543732</v>
       </c>
       <c r="C4">
-        <v>3.807975842935186</v>
+        <v>147.1369575718296</v>
       </c>
       <c r="D4">
-        <v>7.385380029678345</v>
+        <v>7.794174575805664</v>
       </c>
       <c r="E4">
-        <v>1.124221860451826</v>
+        <v>0.697301385337306</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -720,16 +720,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>402.1224253177643</v>
+        <v>377.1240797996521</v>
       </c>
       <c r="C5">
-        <v>8.120850862364099</v>
+        <v>4.488915750976273</v>
       </c>
       <c r="D5">
-        <v>8.27680687904358</v>
+        <v>6.424685859680176</v>
       </c>
       <c r="E5">
-        <v>1.461279364343534</v>
+        <v>0.6204430465207618</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -773,16 +773,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>869.7356701850891</v>
+        <v>747.3299785614014</v>
       </c>
       <c r="C6">
-        <v>44.26379285514578</v>
+        <v>1.435729779805043</v>
       </c>
       <c r="D6">
-        <v>16.79314398765564</v>
+        <v>7.767447471618652</v>
       </c>
       <c r="E6">
-        <v>1.157997056999233</v>
+        <v>0.5263217839837919</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -826,16 +826,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2692.697416543961</v>
+        <v>1503.241074752808</v>
       </c>
       <c r="C7">
-        <v>153.4418528787091</v>
+        <v>8.216632186597469</v>
       </c>
       <c r="D7">
-        <v>20.08386163711548</v>
+        <v>7.806480121612549</v>
       </c>
       <c r="E7">
-        <v>1.176394489121481</v>
+        <v>0.4952123317853763</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -879,16 +879,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>979.8826972961426</v>
+        <v>505.8822907924652</v>
       </c>
       <c r="C8">
-        <v>27.10978567145122</v>
+        <v>2.412524486109187</v>
       </c>
       <c r="D8">
-        <v>17.18815579414368</v>
+        <v>7.771378517150879</v>
       </c>
       <c r="E8">
-        <v>0.53037659947531</v>
+        <v>0.5204026821273751</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -932,16 +932,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1868.212515020371</v>
+        <v>981.9365540504456</v>
       </c>
       <c r="C9">
-        <v>6.047284565886303</v>
+        <v>3.121151172707056</v>
       </c>
       <c r="D9">
-        <v>18.34990372657776</v>
+        <v>7.429174852371216</v>
       </c>
       <c r="E9">
-        <v>1.945805830902262</v>
+        <v>0.5210085033222966</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -985,16 +985,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3742.440726041794</v>
+        <v>1933.971311092377</v>
       </c>
       <c r="C10">
-        <v>10.08778627926592</v>
+        <v>10.17687054758597</v>
       </c>
       <c r="D10">
-        <v>23.71490683555603</v>
+        <v>8.29528088569641</v>
       </c>
       <c r="E10">
-        <v>0.617882023841578</v>
+        <v>0.5526351660262588</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -1038,16 +1038,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>733.9631843090058</v>
+        <v>364.2634794235229</v>
       </c>
       <c r="C11">
-        <v>9.752889495105453</v>
+        <v>10.36124568332492</v>
       </c>
       <c r="D11">
-        <v>18.04124455451965</v>
+        <v>8.166208696365356</v>
       </c>
       <c r="E11">
-        <v>2.026668341601101</v>
+        <v>1.09103588865048</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -1091,16 +1091,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1425.665212965012</v>
+        <v>738.1327583312989</v>
       </c>
       <c r="C12">
-        <v>21.59787926645238</v>
+        <v>17.185077873209</v>
       </c>
       <c r="D12">
-        <v>19.48286547660827</v>
+        <v>8.48124794960022</v>
       </c>
       <c r="E12">
-        <v>0.9652780580455057</v>
+        <v>0.1751275123734161</v>
       </c>
       <c r="F12">
         <v>20</v>
@@ -1144,16 +1144,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2877.978138542175</v>
+        <v>1443.930177211761</v>
       </c>
       <c r="C13">
-        <v>33.30135550412943</v>
+        <v>14.65252708229283</v>
       </c>
       <c r="D13">
-        <v>22.03611583709717</v>
+        <v>7.77112889289856</v>
       </c>
       <c r="E13">
-        <v>2.496534199259842</v>
+        <v>0.734735051367882</v>
       </c>
       <c r="F13">
         <v>20</v>
@@ -1197,16 +1197,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1064.587443208694</v>
+        <v>531.909878540039</v>
       </c>
       <c r="C14">
-        <v>12.24973613157318</v>
+        <v>10.00108584064636</v>
       </c>
       <c r="D14">
-        <v>18.82622060775757</v>
+        <v>8.041028881072998</v>
       </c>
       <c r="E14">
-        <v>1.557137344731039</v>
+        <v>0.4545830724695889</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1250,16 +1250,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2067.778968334198</v>
+        <v>1054.598804473877</v>
       </c>
       <c r="C15">
-        <v>34.50738199522669</v>
+        <v>13.04705813615584</v>
       </c>
       <c r="D15">
-        <v>20.38813481330872</v>
+        <v>7.271795701980591</v>
       </c>
       <c r="E15">
-        <v>0.2976973261216401</v>
+        <v>1.090471930160971</v>
       </c>
       <c r="F15">
         <v>20</v>
@@ -1303,16 +1303,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>4098.578333902359</v>
+        <v>2102.181675291061</v>
       </c>
       <c r="C16">
-        <v>55.42427669638813</v>
+        <v>24.58502204365717</v>
       </c>
       <c r="D16">
-        <v>22.37259693145752</v>
+        <v>7.786889791488647</v>
       </c>
       <c r="E16">
-        <v>2.248584405956028</v>
+        <v>0.891355749180525</v>
       </c>
       <c r="F16">
         <v>20</v>
@@ -1356,16 +1356,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1356.596039676666</v>
+        <v>702.1941849708558</v>
       </c>
       <c r="C17">
-        <v>17.45753337725258</v>
+        <v>9.525333471544933</v>
       </c>
       <c r="D17">
-        <v>20.20234942436218</v>
+        <v>7.351981019973755</v>
       </c>
       <c r="E17">
-        <v>0.700723526523497</v>
+        <v>0.5475775561768333</v>
       </c>
       <c r="F17">
         <v>20</v>
@@ -1409,16 +1409,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2774.804759311676</v>
+        <v>1386.648744726181</v>
       </c>
       <c r="C18">
-        <v>28.39784499988695</v>
+        <v>16.12656439762762</v>
       </c>
       <c r="D18">
-        <v>22.80701861381531</v>
+        <v>7.236619520187378</v>
       </c>
       <c r="E18">
-        <v>2.99355450263551</v>
+        <v>1.124575695069342</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -1462,16 +1462,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5356.676411914826</v>
+        <v>2747.567058753967</v>
       </c>
       <c r="C19">
-        <v>80.95050073209359</v>
+        <v>38.98479698671913</v>
       </c>
       <c r="D19">
-        <v>25.12659869194031</v>
+        <v>8.358428239822388</v>
       </c>
       <c r="E19">
-        <v>2.637285480679805</v>
+        <v>0.9187743836990696</v>
       </c>
       <c r="F19">
         <v>20</v>
@@ -1515,16 +1515,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>769.2456737041473</v>
+        <v>403.0114535331726</v>
       </c>
       <c r="C20">
-        <v>19.10381143442506</v>
+        <v>9.556101852337729</v>
       </c>
       <c r="D20">
-        <v>19.66982178688049</v>
+        <v>7.453378868103028</v>
       </c>
       <c r="E20">
-        <v>0.713803508754051</v>
+        <v>0.6873262598454917</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -1568,16 +1568,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1542.342375993729</v>
+        <v>790.3326588153839</v>
       </c>
       <c r="C21">
-        <v>28.00770570762495</v>
+        <v>15.77419469972016</v>
       </c>
       <c r="D21">
-        <v>21.22058067321777</v>
+        <v>8.232116937637329</v>
       </c>
       <c r="E21">
-        <v>1.421748668362943</v>
+        <v>0.4802826904648368</v>
       </c>
       <c r="F21">
         <v>30</v>
@@ -1621,16 +1621,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>3035.902602291107</v>
+        <v>1556.118911647797</v>
       </c>
       <c r="C22">
-        <v>64.27181256247231</v>
+        <v>22.65195437510166</v>
       </c>
       <c r="D22">
-        <v>23.00688591003418</v>
+        <v>8.390181016921996</v>
       </c>
       <c r="E22">
-        <v>1.251188576880366</v>
+        <v>0.4493497698688949</v>
       </c>
       <c r="F22">
         <v>30</v>
@@ -1674,16 +1674,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1114.169865703583</v>
+        <v>574.2722779750824</v>
       </c>
       <c r="C23">
-        <v>21.67501479369674</v>
+        <v>14.12138459417679</v>
       </c>
       <c r="D23">
-        <v>20.44219408035278</v>
+        <v>8.251580953598022</v>
       </c>
       <c r="E23">
-        <v>1.146077979462136</v>
+        <v>0.0506019854806141</v>
       </c>
       <c r="F23">
         <v>30</v>
@@ -1727,16 +1727,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2185.736706781388</v>
+        <v>1145.251269388199</v>
       </c>
       <c r="C24">
-        <v>51.68832884342411</v>
+        <v>25.60517341490359</v>
       </c>
       <c r="D24">
-        <v>21.05521302223206</v>
+        <v>8.196055459976197</v>
       </c>
       <c r="E24">
-        <v>1.540296024136348</v>
+        <v>0.4691277559583056</v>
       </c>
       <c r="F24">
         <v>30</v>
@@ -1780,16 +1780,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>4368.750047540665</v>
+        <v>2281.5448802948</v>
       </c>
       <c r="C25">
-        <v>89.68013128589108</v>
+        <v>50.18006827834968</v>
       </c>
       <c r="D25">
-        <v>23.69557371139526</v>
+        <v>8.834143114089965</v>
       </c>
       <c r="E25">
-        <v>0.8215986671215267</v>
+        <v>0.08239113847584993</v>
       </c>
       <c r="F25">
         <v>30</v>
@@ -1833,16 +1833,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1458.149303627014</v>
+        <v>758.4038465499877</v>
       </c>
       <c r="C26">
-        <v>26.58867117253022</v>
+        <v>22.60167229475072</v>
       </c>
       <c r="D26">
-        <v>20.85137791633606</v>
+        <v>8.271647024154664</v>
       </c>
       <c r="E26">
-        <v>1.706409462405474</v>
+        <v>0.2250530510250268</v>
       </c>
       <c r="F26">
         <v>30</v>
@@ -1886,16 +1886,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2876.057351350784</v>
+        <v>1477.770034837723</v>
       </c>
       <c r="C27">
-        <v>34.31461913778352</v>
+        <v>26.73667225521547</v>
       </c>
       <c r="D27">
-        <v>21.67716946601868</v>
+        <v>7.51599702835083</v>
       </c>
       <c r="E27">
-        <v>1.715723281017378</v>
+        <v>1.099449395601465</v>
       </c>
       <c r="F27">
         <v>30</v>
@@ -1939,16 +1939,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>4946.953464984894</v>
+        <v>1950.318675088882</v>
       </c>
       <c r="C28">
-        <v>311.6168711934088</v>
+        <v>318.2246469208184</v>
       </c>
       <c r="D28">
-        <v>16.22841792106628</v>
+        <v>2.339125490188599</v>
       </c>
       <c r="E28">
-        <v>3.357347477505025</v>
+        <v>1.576596433059863</v>
       </c>
       <c r="F28">
         <v>30</v>

</xml_diff>